<commit_message>
Add Object3D:: getBiggestAreaScaled() and recalculateBiggerAreaScaled(), etc.
I also updated the implementation of Object3D's scaling setting functions to update the scaling of optional bounding box object too.

Also updated some WriteListCallback().
</commit_message>
<xml_diff>
--- a/PGE/PRRE/docpages/internal/PURE-occluder-selection.xlsx
+++ b/PGE/PRRE/docpages/internal/PURE-occluder-selection.xlsx
@@ -76,9 +76,6 @@
     <t>Set 4</t>
   </si>
   <si>
-    <t>Set 1 - basic PR00FPS scenario</t>
-  </si>
-  <si>
     <t>Set 4 - no map size objects in the scene</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>PRooF88</t>
+  </si>
+  <si>
+    <t>Set 2 - basic PR00FPS scenario</t>
   </si>
 </sst>
 </file>
@@ -356,6 +356,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,9 +423,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -722,14 +722,16 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="4" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -740,18 +742,18 @@
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="19" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -761,13 +763,13 @@
         <f>20*20</f>
         <v>400</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="29" t="s">
+      <c r="C2" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="10"/>
@@ -780,11 +782,11 @@
         <f>3*3</f>
         <v>9</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="23" t="s">
-        <v>21</v>
+      <c r="C3" s="34"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="24" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -795,10 +797,10 @@
         <f t="shared" ref="B4:B9" si="0">3*3</f>
         <v>9</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="24"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="11"/>
       <c r="H4" s="12" t="s">
         <v>11</v>
@@ -821,10 +823,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="24"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="11" t="s">
         <v>17</v>
       </c>
@@ -853,10 +855,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="24"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="11" t="s">
         <v>13</v>
       </c>
@@ -885,10 +887,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="24"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="11" t="s">
         <v>16</v>
       </c>
@@ -917,10 +919,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="24"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="11" t="s">
         <v>14</v>
       </c>
@@ -949,10 +951,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="24"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="11" t="s">
         <v>15</v>
       </c>
@@ -981,12 +983,12 @@
         <f>1*4</f>
         <v>4</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="24"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="11">
         <f>AVEDEV(B2:B16)</f>
@@ -1013,10 +1015,10 @@
         <f t="shared" ref="B11:B16" si="1">1*4</f>
         <v>4</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="4" t="s">
@@ -1026,10 +1028,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="4" t="s">
@@ -1039,12 +1041,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1055,12 +1057,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="38" t="s">
-        <v>24</v>
+      <c r="C14" s="34"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1071,11 +1073,11 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="38"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
@@ -1085,10 +1087,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="24"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
@@ -1098,10 +1100,10 @@
         <f>1*1</f>
         <v>1</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="24"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
@@ -1111,10 +1113,10 @@
         <f t="shared" ref="B18:B33" si="2">1*1</f>
         <v>1</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="24"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
@@ -1124,10 +1126,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="24"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
@@ -1137,10 +1139,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
@@ -1150,10 +1152,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="24"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
@@ -1163,10 +1165,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
@@ -1176,10 +1178,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="24"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
@@ -1189,10 +1191,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="24"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="25"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
@@ -1202,10 +1204,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="24"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="25"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
@@ -1215,10 +1217,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="24"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
@@ -1228,10 +1230,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="24"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="25"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
@@ -1241,10 +1243,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="24"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
@@ -1254,10 +1256,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="24"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
@@ -1267,10 +1269,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="24"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="25"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
@@ -1280,10 +1282,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="24"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
@@ -1293,10 +1295,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="24"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="25"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="6" t="s">
@@ -1306,10 +1308,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="25"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
@@ -1319,10 +1321,10 @@
         <f>20*20</f>
         <v>400</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="16"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
@@ -1332,10 +1334,10 @@
         <f>30*30</f>
         <v>900</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="17"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
@@ -1345,10 +1347,10 @@
         <f>50*50</f>
         <v>2500</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="17"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="6" t="s">
@@ -1358,10 +1360,10 @@
         <f>90*90</f>
         <v>8100</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="18"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>